<commit_message>
refine "hotel voting" use case
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/hotelVoting.xlsx
+++ b/src/main/webapp/WEB-INF/books/hotelVoting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4F74FD-C2CD-C84C-A64D-AB7A67FFE488}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D4673A-DB47-E946-ABA2-21952257A35F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1820" windowWidth="25620" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="1820" windowWidth="25620" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="voting" sheetId="1" r:id="rId1"/>
@@ -1188,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1440,9 +1440,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="37" t="s">
-        <v>5</v>
-      </c>
+      <c r="A18" s="37"/>
       <c r="B18" s="13"/>
       <c r="C18" s="21" t="s">
         <v>29</v>
@@ -1474,7 +1472,9 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="38"/>
+      <c r="A20" s="38" t="s">
+        <v>5</v>
+      </c>
       <c r="B20" s="31"/>
       <c r="C20" s="32" t="s">
         <v>34</v>
@@ -1564,9 +1564,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="37" t="s">
-        <v>5</v>
-      </c>
+      <c r="A26" s="37"/>
       <c r="B26" s="13"/>
       <c r="C26" s="28" t="s">
         <v>42</v>
@@ -1582,7 +1580,9 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="39"/>
+      <c r="A27" s="39" t="s">
+        <v>5</v>
+      </c>
       <c r="B27" s="31"/>
       <c r="C27" s="32" t="s">
         <v>44</v>

</xml_diff>